<commit_message>
Fix spatial relationship bug and remove unnecessary line in process_video function
</commit_message>
<xml_diff>
--- a/old/COCO Dataset Classes.xlsx
+++ b/old/COCO Dataset Classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/md.sazibahmed/Downloads/Thesis/Prototype_up/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thesis\ObjectSense_Voice_Assistant\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08621906-8E2D-324B-A239-15A442A6A920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485319A3-37F6-40CD-97E0-E5EB1BCE0D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{E07CE1F7-7C86-9144-BB3F-DB4CF0B8220A}"/>
+    <workbookView xWindow="21660" yWindow="3390" windowWidth="21600" windowHeight="11295" xr2:uid="{E07CE1F7-7C86-9144-BB3F-DB4CF0B8220A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="227">
   <si>
     <t>ID</t>
   </si>
@@ -609,13 +608,121 @@
   </si>
   <si>
     <t>For Ditection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bench</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> couch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> potted plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dining table</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> microwave</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oven</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> refrigerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> backpack</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> umbrella</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> handbag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> suitcase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sports ball</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fork</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bowl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> remote</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> keyboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cell phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> book</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> scissors</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> teddy bear</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hair drier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> toothbrush</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2526,29 +2633,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FD8F19-BF0C-0D4A-959B-A1D4C7CC9A6C}">
-  <dimension ref="A2:K81"/>
+  <dimension ref="A2:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K30"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41:N46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.375" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
     <col min="8" max="8" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.875" customWidth="1"/>
+    <col min="11" max="11" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="16" t="s">
         <v>109</v>
       </c>
@@ -2565,7 +2672,7 @@
       </c>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="16" t="s">
         <v>110</v>
       </c>
@@ -2588,7 +2695,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="16" t="s">
         <v>111</v>
       </c>
@@ -2610,8 +2717,18 @@
       <c r="K5" s="16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>191</v>
+      </c>
+      <c r="O5" t="str">
+        <f>TRIM(N5)</f>
+        <v>bench</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="16" t="s">
         <v>112</v>
       </c>
@@ -2633,8 +2750,18 @@
       <c r="K6" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" ref="O6:O14" si="0">TRIM(N6)</f>
+        <v>chair</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="16" t="s">
         <v>113</v>
       </c>
@@ -2656,8 +2783,18 @@
       <c r="K7" s="16" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>57</v>
+      </c>
+      <c r="N7" t="s">
+        <v>193</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>couch</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="16" t="s">
         <v>114</v>
       </c>
@@ -2679,8 +2816,18 @@
       <c r="K8" s="16" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
+        <v>194</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>potted plant</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="16" t="s">
         <v>115</v>
       </c>
@@ -2702,8 +2849,18 @@
       <c r="K9" s="16" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
+        <v>195</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>bed</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="16" t="s">
         <v>116</v>
       </c>
@@ -2725,8 +2882,18 @@
       <c r="K10" s="16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>60</v>
+      </c>
+      <c r="N10" t="s">
+        <v>196</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>dining table</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="15" t="s">
         <v>117</v>
       </c>
@@ -2748,8 +2915,18 @@
       <c r="K11" s="16" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>62</v>
+      </c>
+      <c r="N11" t="s">
+        <v>197</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>tv</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="15" t="s">
         <v>118</v>
       </c>
@@ -2771,8 +2948,18 @@
       <c r="K12" s="16" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>68</v>
+      </c>
+      <c r="N12" t="s">
+        <v>198</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>microwave</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="15" t="s">
         <v>119</v>
       </c>
@@ -2794,8 +2981,18 @@
       <c r="K13" s="16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>69</v>
+      </c>
+      <c r="N13" t="s">
+        <v>199</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>oven</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="15" t="s">
         <v>120</v>
       </c>
@@ -2817,8 +3014,18 @@
       <c r="K14" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>72</v>
+      </c>
+      <c r="N14" t="s">
+        <v>200</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>refrigerator</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="17" t="s">
         <v>121</v>
       </c>
@@ -2839,7 +3046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="16" t="s">
         <v>122</v>
       </c>
@@ -2860,7 +3067,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="16" t="s">
         <v>123</v>
       </c>
@@ -2880,7 +3087,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="16" t="s">
         <v>124</v>
       </c>
@@ -2894,7 +3101,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -2908,7 +3115,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="16" t="s">
         <v>126</v>
       </c>
@@ -2922,7 +3129,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="16" t="s">
         <v>127</v>
       </c>
@@ -2935,8 +3142,14 @@
       <c r="K21" s="16" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>15</v>
+      </c>
+      <c r="N21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="16" t="s">
         <v>128</v>
       </c>
@@ -2949,8 +3162,14 @@
       <c r="K22" s="16" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>16</v>
+      </c>
+      <c r="N22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="16" t="s">
         <v>129</v>
       </c>
@@ -2963,8 +3182,14 @@
       <c r="K23" s="16" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="16" t="s">
         <v>130</v>
       </c>
@@ -2977,8 +3202,14 @@
       <c r="K24" s="16" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>25</v>
+      </c>
+      <c r="N24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="16" t="s">
         <v>131</v>
       </c>
@@ -2991,8 +3222,14 @@
       <c r="K25" s="16" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>26</v>
+      </c>
+      <c r="N25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="16" t="s">
         <v>132</v>
       </c>
@@ -3005,8 +3242,14 @@
       <c r="K26" s="16" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>27</v>
+      </c>
+      <c r="N26" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="16" t="s">
         <v>133</v>
       </c>
@@ -3019,8 +3262,14 @@
       <c r="K27" s="16" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="16" t="s">
         <v>134</v>
       </c>
@@ -3033,8 +3282,14 @@
       <c r="K28" s="16" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>32</v>
+      </c>
+      <c r="N28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="16" t="s">
         <v>135</v>
       </c>
@@ -3047,8 +3302,14 @@
       <c r="K29" s="16" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>39</v>
+      </c>
+      <c r="N29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="16" t="s">
         <v>136</v>
       </c>
@@ -3061,8 +3322,14 @@
       <c r="K30" s="16" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>41</v>
+      </c>
+      <c r="N30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="16" t="s">
         <v>137</v>
       </c>
@@ -3072,8 +3339,14 @@
       <c r="H31" s="16" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>42</v>
+      </c>
+      <c r="N31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="16" t="s">
         <v>138</v>
       </c>
@@ -3084,8 +3357,14 @@
         <v>141</v>
       </c>
       <c r="K32" s="19"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>43</v>
+      </c>
+      <c r="N32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="16" t="s">
         <v>139</v>
       </c>
@@ -3096,8 +3375,14 @@
         <v>142</v>
       </c>
       <c r="K33" s="19"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>44</v>
+      </c>
+      <c r="N33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="16" t="s">
         <v>140</v>
       </c>
@@ -3108,8 +3393,14 @@
         <v>143</v>
       </c>
       <c r="K34" s="19"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>45</v>
+      </c>
+      <c r="N34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="16" t="s">
         <v>141</v>
       </c>
@@ -3120,8 +3411,14 @@
         <v>144</v>
       </c>
       <c r="K35" s="19"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>63</v>
+      </c>
+      <c r="N35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="16" t="s">
         <v>142</v>
       </c>
@@ -3132,8 +3429,14 @@
         <v>145</v>
       </c>
       <c r="K36" s="19"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>64</v>
+      </c>
+      <c r="N36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="16" t="s">
         <v>143</v>
       </c>
@@ -3144,8 +3447,14 @@
         <v>146</v>
       </c>
       <c r="K37" s="19"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>65</v>
+      </c>
+      <c r="N37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="16" t="s">
         <v>144</v>
       </c>
@@ -3155,8 +3464,14 @@
       <c r="H38" s="16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>66</v>
+      </c>
+      <c r="N38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="16" t="s">
         <v>145</v>
       </c>
@@ -3167,8 +3482,14 @@
         <v>148</v>
       </c>
       <c r="K39" s="19"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>67</v>
+      </c>
+      <c r="N39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="16" t="s">
         <v>146</v>
       </c>
@@ -3178,8 +3499,14 @@
       <c r="H40" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <v>73</v>
+      </c>
+      <c r="N40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="16" t="s">
         <v>147</v>
       </c>
@@ -3189,8 +3516,14 @@
       <c r="H41" s="16" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <v>74</v>
+      </c>
+      <c r="N41" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="16" t="s">
         <v>148</v>
       </c>
@@ -3200,8 +3533,14 @@
       <c r="H42" s="16" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>75</v>
+      </c>
+      <c r="N42" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="16" t="s">
         <v>149</v>
       </c>
@@ -3211,8 +3550,14 @@
       <c r="H43" s="16" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M43">
+        <v>76</v>
+      </c>
+      <c r="N43" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="16" t="s">
         <v>150</v>
       </c>
@@ -3222,8 +3567,14 @@
       <c r="H44" s="16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>77</v>
+      </c>
+      <c r="N44" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="16" t="s">
         <v>151</v>
       </c>
@@ -3234,8 +3585,14 @@
         <v>154</v>
       </c>
       <c r="K45" s="19"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <v>78</v>
+      </c>
+      <c r="N45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="16" t="s">
         <v>152</v>
       </c>
@@ -3246,8 +3603,14 @@
         <v>155</v>
       </c>
       <c r="K46" s="19"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <v>79</v>
+      </c>
+      <c r="N46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="16" t="s">
         <v>153</v>
       </c>
@@ -3259,7 +3622,7 @@
       </c>
       <c r="K47" s="19"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="A48" s="16" t="s">
         <v>154</v>
       </c>
@@ -3271,7 +3634,7 @@
       </c>
       <c r="K48" s="19"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="16" t="s">
         <v>155</v>
       </c>
@@ -3283,7 +3646,7 @@
       </c>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="16" t="s">
         <v>156</v>
       </c>
@@ -3295,7 +3658,7 @@
       </c>
       <c r="K50" s="19"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="16" t="s">
         <v>157</v>
       </c>
@@ -3307,7 +3670,7 @@
       </c>
       <c r="K51" s="19"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="16" t="s">
         <v>158</v>
       </c>
@@ -3319,7 +3682,7 @@
       </c>
       <c r="K52" s="19"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" s="16" t="s">
         <v>159</v>
       </c>
@@ -3331,7 +3694,7 @@
       </c>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="16" t="s">
         <v>160</v>
       </c>
@@ -3343,7 +3706,7 @@
       </c>
       <c r="K54" s="19"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="16" t="s">
         <v>161</v>
       </c>
@@ -3354,7 +3717,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="16" t="s">
         <v>162</v>
       </c>
@@ -3365,7 +3728,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="16" t="s">
         <v>163</v>
       </c>
@@ -3376,7 +3739,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="17" t="s">
         <v>164</v>
       </c>
@@ -3387,7 +3750,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="17" t="s">
         <v>165</v>
       </c>
@@ -3398,7 +3761,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="17" t="s">
         <v>166</v>
       </c>
@@ -3409,7 +3772,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="17" t="s">
         <v>167</v>
       </c>
@@ -3420,7 +3783,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="17" t="s">
         <v>168</v>
       </c>
@@ -3431,7 +3794,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="17" t="s">
         <v>169</v>
       </c>
@@ -3442,7 +3805,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="17" t="s">
         <v>170</v>
       </c>
@@ -3453,7 +3816,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" s="16" t="s">
         <v>171</v>
       </c>
@@ -3464,7 +3827,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" s="16" t="s">
         <v>172</v>
       </c>
@@ -3475,77 +3838,77 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" s="16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="16" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" s="17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" s="17" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" s="17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" s="16" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" s="16" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" s="16" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" s="16" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="16" t="s">
         <v>187</v>
       </c>
@@ -3568,15 +3931,15 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
     <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3593,7 +3956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -3610,7 +3973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -3627,7 +3990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -3644,7 +4007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -3661,7 +4024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -3678,7 +4041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -3695,7 +4058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -3712,7 +4075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -3729,7 +4092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -3746,7 +4109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -3763,7 +4126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -3780,7 +4143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -3797,7 +4160,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -3814,7 +4177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -3831,7 +4194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -3848,7 +4211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -3865,7 +4228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -3882,7 +4245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -3899,7 +4262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -3916,7 +4279,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -3933,7 +4296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -3950,7 +4313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -3967,7 +4330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -3984,7 +4347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -4001,7 +4364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -4018,7 +4381,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -4035,7 +4398,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -4052,7 +4415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -4069,7 +4432,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -4086,7 +4449,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -4103,7 +4466,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -4120,7 +4483,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -4137,7 +4500,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -4154,7 +4517,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -4171,7 +4534,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -4188,7 +4551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -4205,7 +4568,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -4222,7 +4585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -4239,7 +4602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -4256,7 +4619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -4273,7 +4636,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -4290,7 +4653,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -4307,7 +4670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="12">
         <v>43</v>
       </c>
@@ -4324,7 +4687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="14">
         <v>44</v>
       </c>
@@ -4341,7 +4704,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="14">
         <v>45</v>
       </c>
@@ -4358,7 +4721,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="14">
         <v>46</v>
       </c>
@@ -4375,7 +4738,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="14">
         <v>47</v>
       </c>
@@ -4392,7 +4755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="14">
         <v>48</v>
       </c>
@@ -4409,7 +4772,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="14">
         <v>49</v>
       </c>
@@ -4426,7 +4789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="14">
         <v>50</v>
       </c>
@@ -4443,7 +4806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="14">
         <v>51</v>
       </c>
@@ -4460,7 +4823,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" s="14">
         <v>52</v>
       </c>
@@ -4477,7 +4840,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" s="14">
         <v>53</v>
       </c>
@@ -4494,7 +4857,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" s="14">
         <v>54</v>
       </c>
@@ -4511,7 +4874,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" s="14">
         <v>55</v>
       </c>
@@ -4528,7 +4891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -4545,7 +4908,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -4562,7 +4925,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -4579,7 +4942,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -4596,7 +4959,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -4613,7 +4976,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -4630,7 +4993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" s="13">
         <v>62</v>
       </c>
@@ -4647,7 +5010,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="13">
         <v>63</v>
       </c>
@@ -4664,7 +5027,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="13">
         <v>64</v>
       </c>
@@ -4681,7 +5044,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66" s="13">
         <v>65</v>
       </c>
@@ -4698,7 +5061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" s="12">
         <v>66</v>
       </c>
@@ -4715,7 +5078,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="13">
         <v>67</v>
       </c>
@@ -4732,7 +5095,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" s="13">
         <v>68</v>
       </c>
@@ -4749,7 +5112,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" s="13">
         <v>69</v>
       </c>
@@ -4766,7 +5129,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" s="12">
         <v>70</v>
       </c>
@@ -4783,7 +5146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" s="13">
         <v>71</v>
       </c>
@@ -4800,7 +5163,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" s="13">
         <v>72</v>
       </c>
@@ -4817,7 +5180,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" s="14">
         <v>73</v>
       </c>
@@ -4834,7 +5197,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="14">
         <v>74</v>
       </c>
@@ -4851,7 +5214,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" s="14">
         <v>75</v>
       </c>
@@ -4868,7 +5231,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" s="14">
         <v>76</v>
       </c>
@@ -4885,7 +5248,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" s="14">
         <v>77</v>
       </c>
@@ -4902,7 +5265,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" s="13">
         <v>78</v>
       </c>
@@ -4919,7 +5282,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" s="13">
         <v>79</v>
       </c>
@@ -4936,7 +5299,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" s="13">
         <v>80</v>
       </c>
@@ -4953,7 +5316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" s="13">
         <v>81</v>
       </c>
@@ -4970,7 +5333,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" s="13">
         <v>82</v>
       </c>
@@ -4987,7 +5350,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84" s="13">
         <v>83</v>
       </c>
@@ -5004,7 +5367,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85" s="14">
         <v>84</v>
       </c>
@@ -5021,7 +5384,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="14">
         <v>85</v>
       </c>
@@ -5038,7 +5401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87" s="14">
         <v>86</v>
       </c>
@@ -5055,7 +5418,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" s="14">
         <v>87</v>
       </c>
@@ -5072,7 +5435,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" s="14">
         <v>88</v>
       </c>
@@ -5089,7 +5452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" s="14">
         <v>89</v>
       </c>
@@ -5106,7 +5469,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" s="14">
         <v>90</v>
       </c>
@@ -5123,7 +5486,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" s="14">
         <v>91</v>
       </c>
@@ -5140,436 +5503,436 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="18">
       <c r="A93" s="3"/>
     </row>
-    <row r="95" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="18">
       <c r="A95" s="3"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" s="4"/>
     </row>
-    <row r="99" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="18">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="18">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" ht="18">
       <c r="A113" s="3"/>
     </row>
-    <row r="115" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" ht="18">
       <c r="A115" s="3"/>
     </row>
-    <row r="117" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" ht="18">
       <c r="A117" s="5"/>
     </row>
-    <row r="119" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" ht="18">
       <c r="A119" s="3"/>
     </row>
-    <row r="121" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" ht="18">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" ht="18">
       <c r="A122" s="5"/>
     </row>
-    <row r="124" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" ht="18">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" ht="18">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" ht="18">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" ht="18">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" ht="18">
       <c r="A128" s="3"/>
     </row>
-    <row r="130" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" ht="18">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" ht="18">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" ht="18">
       <c r="A132" s="6"/>
     </row>
-    <row r="134" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" ht="23.25">
       <c r="A134" s="7"/>
     </row>
-    <row r="135" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" ht="18">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1">
       <c r="A136" s="4"/>
     </row>
-    <row r="139" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" ht="18">
       <c r="A139" s="3"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" s="4"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="4"/>
     </row>
-    <row r="145" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" ht="18">
       <c r="A145" s="3"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1">
       <c r="A147" s="4"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" s="4"/>
     </row>
-    <row r="151" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" ht="18">
       <c r="A151" s="3"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1">
       <c r="A153" s="4"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1">
       <c r="A154" s="4"/>
     </row>
-    <row r="157" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" ht="18">
       <c r="A157" s="3"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1">
       <c r="A159" s="4"/>
     </row>
-    <row r="160" spans="1:1" ht="19" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" ht="18.75">
       <c r="A160" s="8"/>
     </row>
-    <row r="163" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" ht="18">
       <c r="A163" s="3"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1">
       <c r="A166" s="4"/>
     </row>
-    <row r="169" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" ht="18">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" ht="18">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1">
       <c r="A171" s="4"/>
     </row>
-    <row r="174" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" ht="18">
       <c r="A174" s="3"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1">
       <c r="A176" s="4"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1">
       <c r="A177" s="4"/>
     </row>
-    <row r="180" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" ht="18">
       <c r="A180" s="3"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1">
       <c r="A182" s="4"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1">
       <c r="A183" s="4"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1">
       <c r="A184" s="4"/>
     </row>
-    <row r="187" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" ht="18">
       <c r="A187" s="3"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1">
       <c r="A189" s="4"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1">
       <c r="A190" s="4"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1">
       <c r="A193" s="4"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1">
       <c r="A195" s="4"/>
     </row>
-    <row r="196" spans="1:1" ht="19" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" ht="18.75">
       <c r="A196" s="8"/>
     </row>
-    <row r="199" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" ht="18">
       <c r="A199" s="3"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1">
       <c r="A201" s="4"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1">
       <c r="A202" s="4"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1">
       <c r="A203" s="4"/>
     </row>
-    <row r="206" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" ht="18">
       <c r="A206" s="3"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1">
       <c r="A208" s="4"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1">
       <c r="A209" s="4"/>
     </row>
-    <row r="212" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" ht="18">
       <c r="A212" s="3"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1">
       <c r="A214" s="4"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1">
       <c r="A215" s="4"/>
     </row>
-    <row r="218" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" ht="18">
       <c r="A218" s="3"/>
     </row>
-    <row r="219" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" ht="18">
       <c r="A219" s="3"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1">
       <c r="A220" s="4"/>
     </row>
-    <row r="223" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" ht="18">
       <c r="A223" s="3"/>
     </row>
-    <row r="224" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" ht="18">
       <c r="A224" s="3"/>
     </row>
-    <row r="225" spans="1:1" ht="19" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" ht="18.75">
       <c r="A225" s="8"/>
     </row>
-    <row r="228" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" ht="18">
       <c r="A228" s="3"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1">
       <c r="A230" s="4"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1">
       <c r="A231" s="4"/>
     </row>
-    <row r="234" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" ht="18">
       <c r="A234" s="3"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1">
       <c r="A236" s="4"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1">
       <c r="A237" s="4"/>
     </row>
-    <row r="240" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" ht="18">
       <c r="A240" s="3"/>
     </row>
-    <row r="241" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" ht="18">
       <c r="A241" s="3"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1">
       <c r="A243" s="4"/>
     </row>
-    <row r="244" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" ht="17.25">
       <c r="A244" s="9"/>
     </row>
-    <row r="246" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" ht="18">
       <c r="A246" s="3"/>
     </row>
-    <row r="248" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" ht="18">
       <c r="A248" s="3"/>
     </row>
-    <row r="250" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" ht="18">
       <c r="A250" s="3"/>
     </row>
-    <row r="252" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" ht="18">
       <c r="A252" s="3"/>
     </row>
-    <row r="254" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" ht="18">
       <c r="A254" s="3"/>
     </row>
-    <row r="256" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" ht="18">
       <c r="A256" s="3"/>
     </row>
-    <row r="258" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" ht="18">
       <c r="A258" s="3"/>
     </row>
-    <row r="260" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" ht="18">
       <c r="A260" s="3"/>
     </row>
-    <row r="262" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" ht="17.25">
       <c r="A262" s="10"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1">
       <c r="A264" s="4"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1">
       <c r="A265" s="4"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1">
       <c r="A266" s="4"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1">
       <c r="A267" s="4"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1">
       <c r="A268" s="4"/>
     </row>
-    <row r="270" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" ht="17.25">
       <c r="A270" s="10"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1">
       <c r="A272" s="4"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1">
       <c r="A273" s="4"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1">
       <c r="A274" s="4"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1">
       <c r="A275" s="4"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1">
       <c r="A276" s="4"/>
     </row>
-    <row r="278" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" ht="17.25">
       <c r="A278" s="10"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1">
       <c r="A280" s="4"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1">
       <c r="A281" s="4"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1">
       <c r="A282" s="4"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1">
       <c r="A283" s="4"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1">
       <c r="A284" s="4"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1">
       <c r="A285" s="4"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1">
       <c r="A286" s="4"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1">
       <c r="A287" s="4"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1">
       <c r="A288" s="4"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1">
       <c r="A289" s="4"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1">
       <c r="A290" s="4"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1">
       <c r="A291" s="4"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1">
       <c r="A292" s="4"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1">
       <c r="A293" s="4"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1">
       <c r="A294" s="4"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1">
       <c r="A295" s="4"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1">
       <c r="A296" s="4"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1">
       <c r="A297" s="4"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1">
       <c r="A298" s="4"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1">
       <c r="A299" s="4"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1">
       <c r="A300" s="4"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1">
       <c r="A301" s="4"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1">
       <c r="A302" s="4"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1">
       <c r="A303" s="4"/>
     </row>
   </sheetData>

</xml_diff>